<commit_message>
Update Dinamica model to source scripts, Update simulation control procedure
</commit_message>
<xml_diff>
--- a/Tools/LULC_class_aggregation.xlsx
+++ b/Tools/LULC_class_aggregation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LULCC_CH\Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bblack\switchdrive\C.3_Modelling\LULCC_CH_HPC\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AFE05E-97B3-4278-AD2A-D844CE6A9FEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7150C2-BB2F-41DF-8002-A52E3EBAB9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6480" xr2:uid="{461A3D3D-11BC-4F5B-AC99-BB9F607AA1FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{461A3D3D-11BC-4F5B-AC99-BB9F607AA1FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -877,7 +877,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1213,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C81117-CCD0-4C70-9A30-E4F720811826}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Squashed commit from upstream/hpc
</commit_message>
<xml_diff>
--- a/Tools/LULC_class_aggregation.xlsx
+++ b/Tools/LULC_class_aggregation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bblack\switchdrive\C.3_Modelling\LULCC_CH_HPC\Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LULCC_CH_Ensemble\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7150C2-BB2F-41DF-8002-A52E3EBAB9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD4D755-52C1-4D61-A62D-2222CD546612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{461A3D3D-11BC-4F5B-AC99-BB9F607AA1FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{461A3D3D-11BC-4F5B-AC99-BB9F607AA1FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1213,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C81117-CCD0-4C70-9A30-E4F720811826}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>